<commit_message>
Cambio de nombre del archivo resultado para vincular con power bi
</commit_message>
<xml_diff>
--- a/Data/Pedido de compra (purchase.order) (1).xlsx
+++ b/Data/Pedido de compra (purchase.order) (1).xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrios\Desktop\ReporteGeneral\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70BF4AC-CF70-46DA-B4BF-C7624647A1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24179BB6-1DCD-4946-BDA2-74F8E89918DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -485,7 +496,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>